<commit_message>
More work, mostly on adventures
</commit_message>
<xml_diff>
--- a/SupersNew/characters/NPC Sheet.xlsx
+++ b/SupersNew/characters/NPC Sheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="211">
   <si>
     <t>Name</t>
   </si>
@@ -246,12 +246,6 @@
   </si>
   <si>
     <t>Effect</t>
-  </si>
-  <si>
-    <t>Bonuses:</t>
-  </si>
-  <si>
-    <t>Day Job:</t>
   </si>
   <si>
     <t>Initiative</t>
@@ -1142,7 +1136,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1147,7 @@
     <col min="4" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1174,7 +1168,7 @@
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -1182,14 +1176,14 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -1245,9 +1239,7 @@
       <c r="G6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1269,9 +1261,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1407,7 +1397,7 @@
     </row>
     <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4">
         <f>_xlfn.CEILING.MATH($B$7*0.5) + _xlfn.CEILING.MATH($B$12 *0.5) + $B$10 + 8</f>
@@ -1415,18 +1405,18 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4">
         <v>6</v>
@@ -1440,7 +1430,7 @@
     </row>
     <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4">
         <f xml:space="preserve"> _xlfn.FLOOR.MATH(C11+C9)</f>
@@ -1499,7 +1489,7 @@
         <v>69</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>70</v>
@@ -1561,37 +1551,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1606,97 +1596,97 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -1706,97 +1696,97 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1847,12 +1837,12 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+2+8</f>
@@ -1880,7 +1870,7 @@
     </row>
     <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+3+8</f>
@@ -1910,7 +1900,7 @@
     </row>
     <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
@@ -2148,7 +2138,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+0+8</f>
@@ -2238,7 +2228,7 @@
     </row>
     <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+2+8</f>
@@ -2506,7 +2496,7 @@
     </row>
     <row r="24" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
@@ -2624,7 +2614,7 @@
     </row>
     <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
@@ -2654,7 +2644,7 @@
     </row>
     <row r="29" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
@@ -2714,7 +2704,7 @@
     </row>
     <row r="31" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
@@ -2744,7 +2734,7 @@
     </row>
     <row r="32" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+0+8</f>
@@ -2774,7 +2764,7 @@
     </row>
     <row r="33" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C12+0+8</f>
@@ -2804,7 +2794,7 @@
     </row>
     <row r="34" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C8+3+8</f>
@@ -3130,7 +3120,7 @@
     </row>
     <row r="45" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+3+8</f>
@@ -3160,7 +3150,7 @@
     </row>
     <row r="46" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C9+1+8</f>
@@ -3220,7 +3210,7 @@
     </row>
     <row r="48" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+1+8</f>
@@ -3289,10 +3279,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -3309,262 +3299,262 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>135</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Working on this week's shennanigans
</commit_message>
<xml_diff>
--- a/SupersNew/characters/NPC Sheet.xlsx
+++ b/SupersNew/characters/NPC Sheet.xlsx
@@ -16,6 +16,8 @@
     <sheet name="Power Sets" sheetId="4" r:id="rId2"/>
     <sheet name="Fighting Profiles" sheetId="2" r:id="rId3"/>
     <sheet name="Day Jobs" sheetId="3" r:id="rId4"/>
+    <sheet name="PowersTest" sheetId="5" r:id="rId5"/>
+    <sheet name="Character Sheet Test" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="279">
   <si>
     <t>Name</t>
   </si>
@@ -536,6 +538,24 @@
     <t>+1 W, +1 C</t>
   </si>
   <si>
+    <t>Job:</t>
+  </si>
+  <si>
+    <t>Stats:</t>
+  </si>
+  <si>
+    <t>Sample Proficiencies:</t>
+  </si>
+  <si>
+    <t>Boon 1:</t>
+  </si>
+  <si>
+    <t>Boon 2:</t>
+  </si>
+  <si>
+    <t>Boon 3:</t>
+  </si>
+  <si>
     <t>Power Sets</t>
   </si>
   <si>
@@ -666,13 +686,232 @@
   </si>
   <si>
     <t>Telekinesis</t>
+  </si>
+  <si>
+    <t>Rng</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>Ars</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>5/</t>
+  </si>
+  <si>
+    <t>1 tgt</t>
+  </si>
+  <si>
+    <t>Breast Plate</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Chariot</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Self +1</t>
+  </si>
+  <si>
+    <t>Cleave</t>
+  </si>
+  <si>
+    <t>Vm</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Favor of the Gods</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Hero’s Shout</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Horn</t>
+  </si>
+  <si>
+    <t>0”</t>
+  </si>
+  <si>
+    <t>7 rad</t>
+  </si>
+  <si>
+    <t>Improved Charge</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>3/</t>
+  </si>
+  <si>
+    <t>Offensive Stance</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Sweep</t>
+  </si>
+  <si>
+    <t>10P</t>
+  </si>
+  <si>
+    <t>2-3 tgt</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>20P</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Knock(1)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pierce(2)</t>
+  </si>
+  <si>
+    <t>2d8 + Skill Physical Damage</t>
+  </si>
+  <si>
+    <t>Armor 3/3/0</t>
+  </si>
+  <si>
+    <t>12' Running</t>
+  </si>
+  <si>
+    <t>One passenger allowed</t>
+  </si>
+  <si>
+    <t>Cleave(11)</t>
+  </si>
+  <si>
+    <t>When you down a foe with a melee attack, you may spend an energy to make a ½ move and attack a second time. Downing an opponent with an x or more on your attack die waives the energy cost</t>
+  </si>
+  <si>
+    <t>+2 to all saving throws</t>
+  </si>
+  <si>
+    <t>Armor 2/2/2</t>
+  </si>
+  <si>
+    <t>Mental Saves +1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+2d3 to Muscle and Skill</t>
+    </r>
+  </si>
+  <si>
+    <t>Allies +1 accuracy</t>
+  </si>
+  <si>
+    <t>Allies +2 damage</t>
+  </si>
+  <si>
+    <t>Allies +2 saves</t>
+  </si>
+  <si>
+    <t>You take no penalty when charging</t>
+  </si>
+  <si>
+    <t>4/4/- &amp; 4d6 Entangle</t>
+  </si>
+  <si>
+    <t>You get +1 to hit and +2 damage but take -1 to all defenses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+2 Block</t>
+    </r>
+  </si>
+  <si>
+    <t>Bonus Block(1)</t>
+  </si>
+  <si>
+    <t>May block incoming missiles</t>
+  </si>
+  <si>
+    <t>You may take a -3 accuracy to make a melee attack against two adjacent enemies</t>
+  </si>
+  <si>
+    <t>2d8 + Muscle Physical Damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,6 +946,31 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -728,7 +992,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -768,20 +1032,31 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,18 +1081,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,6 +1142,167 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{690BC951-4BAC-7540-AE5F-EBF8BEB8C814}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7442200" y="177800"/>
+          <a:ext cx="4546600" cy="889000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>To Use, fill in your stats in the highlighted colum, then select your fighting profile from the drop down. (Both highlighted in blue).</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> You can also select your power sets and your day job (again in blue). Powers are manual for the time being.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E211944-C884-7143-B7C9-6DB1303AC3AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3822700" y="4610100"/>
+          <a:ext cx="1193800" cy="520700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Highlight</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> your selected perk</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1133,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1616,7 @@
     <col min="4" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1155,11 +1624,11 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
@@ -1170,14 +1639,12 @@
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
     </row>
@@ -1185,11 +1652,11 @@
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1256,9 +1723,9 @@
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="4" t="e">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,2,FALSE))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1278,9 +1745,9 @@
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="4" t="e">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,3,FALSE))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1300,9 +1767,9 @@
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="4" t="e">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,4,FALSE))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1322,9 +1789,9 @@
       <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="4" t="e">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,5,FALSE))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1334,19 +1801,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="4" t="e">
         <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,6,FALSE))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1400,15 +1867,15 @@
         <v>72</v>
       </c>
       <c r="B15" s="4">
-        <f>_xlfn.CEILING.MATH($B$7*0.5) + _xlfn.CEILING.MATH($B$12 *0.5) + $B$10 + 8</f>
-        <v>28</v>
+        <f>_xlfn.CEILING.MATH(B7*(0.5)) + _xlfn.CEILING.MATH(B11*(0.5))+8+B10</f>
+        <v>29</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="9" t="s">
         <v>77</v>
       </c>
@@ -1425,7 +1892,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1440,75 +1907,65 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="4"/>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+    <row r="20" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G16:G17"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="E15:F15"/>
@@ -1528,7 +1985,7 @@
           <x14:formula1>
             <xm:f>'Power Sets'!$A$2:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 C3</xm:sqref>
+          <xm:sqref>B3:C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1551,37 +2008,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1596,97 +2053,97 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -1696,17 +2153,17 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -1716,77 +2173,77 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1854,7 +2311,7 @@
       </c>
       <c r="D2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -1862,7 +2319,7 @@
       </c>
       <c r="F2" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1874,11 +2331,11 @@
       </c>
       <c r="B3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="C3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -1886,11 +2343,11 @@
       </c>
       <c r="E3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F3" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1912,7 +2369,7 @@
       </c>
       <c r="D4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="E4" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+0+8</f>
@@ -2006,11 +2463,11 @@
       </c>
       <c r="E7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F7" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -2054,7 +2511,7 @@
       </c>
       <c r="B9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="C9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C8+3+8</f>
@@ -2066,7 +2523,7 @@
       </c>
       <c r="E9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F9" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+1+8</f>
@@ -2142,11 +2599,11 @@
       </c>
       <c r="B12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+0+8</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="C12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D12" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C9+3+8</f>
@@ -2240,7 +2697,7 @@
       </c>
       <c r="D15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
@@ -2248,7 +2705,7 @@
       </c>
       <c r="F15" s="11">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2274,7 +2731,7 @@
       </c>
       <c r="E16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F16" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+5+8</f>
@@ -2292,11 +2749,11 @@
       </c>
       <c r="B17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="C17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="D17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -2304,11 +2761,11 @@
       </c>
       <c r="E17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F17" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -2410,11 +2867,11 @@
       </c>
       <c r="B21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C7+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="C21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -2422,11 +2879,11 @@
       </c>
       <c r="E21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F21" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2448,15 +2905,15 @@
       </c>
       <c r="D22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="E22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F22" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2564,19 +3021,19 @@
       </c>
       <c r="C26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F26" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2588,15 +3045,15 @@
       </c>
       <c r="B27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C7+0+8</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="C27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="E27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+3+8</f>
@@ -2604,7 +3061,7 @@
       </c>
       <c r="F27" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -2626,7 +3083,7 @@
       </c>
       <c r="D28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="E28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -2634,7 +3091,7 @@
       </c>
       <c r="F28" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -2652,19 +3109,19 @@
       </c>
       <c r="C29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="D29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F29" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C12+'Character Sheet'!C11+4+8</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -2690,7 +3147,7 @@
       </c>
       <c r="E30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+4+8</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="F30" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+0+8</f>
@@ -2724,7 +3181,7 @@
       </c>
       <c r="F31" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C10+'Character Sheet'!C11+0+8</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2742,19 +3199,19 @@
       </c>
       <c r="C32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="D32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="E32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F32" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -2842,7 +3299,7 @@
       </c>
       <c r="F35" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -2902,7 +3359,7 @@
       </c>
       <c r="F37" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+0+8</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2958,7 +3415,7 @@
       </c>
       <c r="E39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F39" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C12+3+8</f>
@@ -3044,15 +3501,15 @@
       </c>
       <c r="D42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+4+8</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="E42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F42" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C12+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -3124,7 +3581,7 @@
       </c>
       <c r="B45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="C45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C8+2+8</f>
@@ -3132,7 +3589,7 @@
       </c>
       <c r="D45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C9+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="E45" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C2+'Character Sheet'!C8+2+8</f>
@@ -3158,11 +3615,11 @@
       </c>
       <c r="C46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="D46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C13+'Character Sheet'!C9+3+8</f>
@@ -3170,7 +3627,7 @@
       </c>
       <c r="F46" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -3214,7 +3671,7 @@
       </c>
       <c r="B48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C7+'Character Sheet'!C11+1+8</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="C48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C8+'Character Sheet'!C9+2+8</f>
@@ -3222,15 +3679,15 @@
       </c>
       <c r="D48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C9+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C8+3+8</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="F48" s="4">
         <f xml:space="preserve"> 'Character Sheet'!C11+'Character Sheet'!C13+2+8</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -3281,11 +3738,11 @@
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
@@ -3707,4 +4164,1120 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="28">
+        <v>20</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="28">
+        <v>1</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="28">
+        <v>4</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="18">
+        <v>20</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="28">
+        <v>20</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="H8" s="28">
+        <v>1</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D10" s="28">
+        <v>10</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="189" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="18">
+        <v>20</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" s="28">
+        <v>20</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" s="18">
+        <v>20</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="28">
+        <v>20</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="H16" s="28">
+        <v>2</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="18">
+        <v>10</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="18">
+        <v>20</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="F20" s="18">
+        <v>0</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="18">
+        <v>4</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="54" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="18">
+        <v>10</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" s="28">
+        <v>20</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H22" s="28">
+        <v>2</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="H25" s="18">
+        <v>1</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F26" s="18">
+        <v>0</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="H26" s="18">
+        <v>3</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G16:G18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" ref="C7:C13" si="0">(B7 - 10)/2</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4">
+        <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,2,FALSE))</f>
+        <v>10</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4">
+        <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,3,FALSE))</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4">
+        <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,4,FALSE))</f>
+        <v>10</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4">
+        <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,5,FALSE))</f>
+        <v>10</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4">
+        <f>_xlfn.FLOOR.MATH(VLOOKUP(G2,'Fighting Profiles'!A2:F48,6,FALSE))</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="4">
+        <f>(_xlfn.CEILING.MATH(B7*(0.5)+B12*(0.5))+8+B10)</f>
+        <v>28</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="4">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="4">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH(C11+C9)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f>VLOOKUP(B19,'Day Jobs'!A3:F15,2,FALSE)</f>
+        <v>+1 W, +1 C</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="31" t="str">
+        <f>VLOOKUP(B19,'Day Jobs'!A3:F15,3,FALSE)</f>
+        <v>Improvise (CW), Perform (CW), Lie (CW), Crafty (RS)</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="29" t="str">
+        <f>VLOOKUP(B19,'Day Jobs'!A3:F15,4,FALSE)</f>
+        <v>Big Personality</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="29" t="str">
+        <f>VLOOKUP(B19,'Day Jobs'!A3:F15,5,FALSE)</f>
+        <v>Quick Change</v>
+      </c>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="29" t="str">
+        <f>VLOOKUP(B19,'Day Jobs'!A3:F15,6,FALSE)</f>
+        <v>Star Material</v>
+      </c>
+      <c r="C24" s="29"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Power Sets'!$A$2:$A$48</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Day Jobs'!$A$4:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Fighting Profiles'!$A$2:$A$48</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>